<commit_message>
raw data (from Wikipedia)
</commit_message>
<xml_diff>
--- a/elevation extremes.xlsx
+++ b/elevation extremes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prescott\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prescott\Documents\R Projects\mountain.trivia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$G$507</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6654" uniqueCount="1883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6996" uniqueCount="1869">
   <si>
     <t> Afghanistan</t>
   </si>
@@ -7731,48 +7732,6 @@
   </si>
   <si>
     <t>0 [22]</t>
-  </si>
-  <si>
-    <t>Aconcagua</t>
-  </si>
-  <si>
-    <t>Mount Kosciuszko</t>
-  </si>
-  <si>
-    <t>Deep Lake, Vestfold Hills</t>
-  </si>
-  <si>
-    <t>Laguna del Carbón</t>
-  </si>
-  <si>
-    <t>Ojos del Salado</t>
-  </si>
-  <si>
-    <t>Mount Everest</t>
-  </si>
-  <si>
-    <t>Dead Sea</t>
-  </si>
-  <si>
-    <t>Denali</t>
-  </si>
-  <si>
-    <t>Sariqarnish Kuli</t>
-  </si>
-  <si>
-    <t>Badwater Basin</t>
-  </si>
-  <si>
-    <t>Vpadina Akchanaya</t>
-  </si>
-  <si>
-    <t>Teide on Tenerife</t>
-  </si>
-  <si>
-    <t>Mount Paget</t>
-  </si>
-  <si>
-    <t>Mount Elbrus</t>
   </si>
 </sst>
 </file>
@@ -40848,7 +40807,7 @@
   <dimension ref="A1:F254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D254" sqref="A1:D254"/>
+      <selection activeCell="F1" sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45948,21 +45907,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D254"/>
+  <dimension ref="A1:F254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B175" sqref="B175"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="108.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1485</v>
       </c>
@@ -45975,8 +45936,14 @@
       <c r="D1" t="s">
         <v>1488</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -45989,8 +45956,14 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -46003,8 +45976,14 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -46017,8 +45996,14 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -46031,8 +46016,14 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -46045,8 +46036,14 @@
       <c r="D6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>1577</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -46059,8 +46056,14 @@
       <c r="D7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -46073,8 +46076,14 @@
       <c r="D8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -46085,10 +46094,16 @@
         <v>1499</v>
       </c>
       <c r="D9" t="s">
-        <v>1871</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1385</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -46101,22 +46116,34 @@
       <c r="D10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>1869</v>
+        <v>1387</v>
       </c>
       <c r="C11" t="s">
         <v>1501</v>
       </c>
       <c r="D11" t="s">
-        <v>1872</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1388</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -46129,8 +46156,14 @@
       <c r="D12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -46143,8 +46176,14 @@
       <c r="D13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1389</v>
       </c>
@@ -46157,13 +46196,19 @@
       <c r="D14" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>1870</v>
+        <v>1390</v>
       </c>
       <c r="C15" t="s">
         <v>1505</v>
@@ -46171,8 +46216,14 @@
       <c r="D15" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -46185,8 +46236,14 @@
       <c r="D16" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -46199,8 +46256,14 @@
       <c r="D17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -46213,8 +46276,14 @@
       <c r="D18" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -46227,8 +46296,14 @@
       <c r="D19" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -46241,8 +46316,14 @@
       <c r="D20" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -46255,8 +46336,14 @@
       <c r="D21" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -46269,8 +46356,14 @@
       <c r="D22" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>143</v>
       </c>
@@ -46283,8 +46376,14 @@
       <c r="D23" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>153</v>
       </c>
@@ -46297,8 +46396,14 @@
       <c r="D24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -46311,8 +46416,14 @@
       <c r="D25" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>162</v>
       </c>
@@ -46325,8 +46436,14 @@
       <c r="D26" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>166</v>
       </c>
@@ -46339,8 +46456,14 @@
       <c r="D27" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>1752</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>175</v>
       </c>
@@ -46353,8 +46476,14 @@
       <c r="D28" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -46367,8 +46496,14 @@
       <c r="D29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>186</v>
       </c>
@@ -46381,8 +46516,14 @@
       <c r="D30" t="s">
         <v>1392</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>195</v>
       </c>
@@ -46395,8 +46536,14 @@
       <c r="D31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>199</v>
       </c>
@@ -46409,8 +46556,14 @@
       <c r="D32" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>205</v>
       </c>
@@ -46423,8 +46576,14 @@
       <c r="D33" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>209</v>
       </c>
@@ -46437,8 +46596,14 @@
       <c r="D34" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>214</v>
       </c>
@@ -46451,8 +46616,14 @@
       <c r="D35" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -46465,8 +46636,14 @@
       <c r="D36" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>1757</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>228</v>
       </c>
@@ -46479,8 +46656,14 @@
       <c r="D37" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>1759</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>237</v>
       </c>
@@ -46493,8 +46676,14 @@
       <c r="D38" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>242</v>
       </c>
@@ -46507,8 +46696,14 @@
       <c r="D39" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>247</v>
       </c>
@@ -46521,8 +46716,14 @@
       <c r="D40" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>253</v>
       </c>
@@ -46535,8 +46736,14 @@
       <c r="D41" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>257</v>
       </c>
@@ -46549,8 +46756,14 @@
       <c r="D42" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>261</v>
       </c>
@@ -46563,8 +46776,14 @@
       <c r="D43" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>1761</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>270</v>
       </c>
@@ -46577,13 +46796,19 @@
       <c r="D44" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>279</v>
       </c>
       <c r="B45" t="s">
-        <v>1873</v>
+        <v>1395</v>
       </c>
       <c r="C45" t="s">
         <v>1535</v>
@@ -46591,13 +46816,19 @@
       <c r="D45" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1396</v>
       </c>
       <c r="B46" t="s">
-        <v>1874</v>
+        <v>1397</v>
       </c>
       <c r="C46" t="s">
         <v>1536</v>
@@ -46605,8 +46836,14 @@
       <c r="D46" t="s">
         <v>1398</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -46619,8 +46856,14 @@
       <c r="D47" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1399</v>
       </c>
@@ -46633,8 +46876,14 @@
       <c r="D48" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>300</v>
       </c>
@@ -46647,8 +46896,14 @@
       <c r="D49" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>303</v>
       </c>
@@ -46661,8 +46916,14 @@
       <c r="D50" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>308</v>
       </c>
@@ -46675,8 +46936,14 @@
       <c r="D51" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>312</v>
       </c>
@@ -46689,8 +46956,14 @@
       <c r="D52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>316</v>
       </c>
@@ -46703,8 +46976,14 @@
       <c r="D53" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>320</v>
       </c>
@@ -46717,8 +46996,14 @@
       <c r="D54" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1403</v>
       </c>
@@ -46731,8 +47016,14 @@
       <c r="D55" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>326</v>
       </c>
@@ -46745,8 +47036,14 @@
       <c r="D56" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>330</v>
       </c>
@@ -46759,8 +47056,14 @@
       <c r="D57" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>335</v>
       </c>
@@ -46773,8 +47076,14 @@
       <c r="D58" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>339</v>
       </c>
@@ -46787,8 +47096,14 @@
       <c r="D59" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>343</v>
       </c>
@@ -46801,8 +47116,14 @@
       <c r="D60" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>347</v>
       </c>
@@ -46815,8 +47136,14 @@
       <c r="D61" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>352</v>
       </c>
@@ -46829,8 +47156,14 @@
       <c r="D62" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>359</v>
       </c>
@@ -46843,8 +47176,14 @@
       <c r="D63" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>1768</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -46857,8 +47196,14 @@
       <c r="D64" t="s">
         <v>1404</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>377</v>
       </c>
@@ -46871,8 +47216,14 @@
       <c r="D65" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>381</v>
       </c>
@@ -46885,8 +47236,14 @@
       <c r="D66" t="s">
         <v>1406</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>390</v>
       </c>
@@ -46899,8 +47256,14 @@
       <c r="D67" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>395</v>
       </c>
@@ -46913,8 +47276,14 @@
       <c r="D68" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>404</v>
       </c>
@@ -46927,8 +47296,14 @@
       <c r="D69" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>408</v>
       </c>
@@ -46941,8 +47316,14 @@
       <c r="D70" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>412</v>
       </c>
@@ -46955,8 +47336,14 @@
       <c r="D71" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>421</v>
       </c>
@@ -46969,8 +47356,14 @@
       <c r="D72" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>426</v>
       </c>
@@ -46983,8 +47376,14 @@
       <c r="D73" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>1777</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>435</v>
       </c>
@@ -46997,8 +47396,14 @@
       <c r="D74" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>444</v>
       </c>
@@ -47011,8 +47416,14 @@
       <c r="D75" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>448</v>
       </c>
@@ -47025,8 +47436,14 @@
       <c r="D76" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>452</v>
       </c>
@@ -47039,8 +47456,14 @@
       <c r="D77" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>456</v>
       </c>
@@ -47053,8 +47476,14 @@
       <c r="D78" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>458</v>
       </c>
@@ -47067,8 +47496,14 @@
       <c r="D79" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>1781</v>
+      </c>
+      <c r="F79" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>467</v>
       </c>
@@ -47081,8 +47516,14 @@
       <c r="D80" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>471</v>
       </c>
@@ -47095,8 +47536,14 @@
       <c r="D81" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>475</v>
       </c>
@@ -47109,8 +47556,14 @@
       <c r="D82" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>477</v>
       </c>
@@ -47123,8 +47576,14 @@
       <c r="D83" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>481</v>
       </c>
@@ -47137,8 +47596,14 @@
       <c r="D84" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>486</v>
       </c>
@@ -47151,8 +47616,14 @@
       <c r="D85" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>490</v>
       </c>
@@ -47165,8 +47636,14 @@
       <c r="D86" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>498</v>
       </c>
@@ -47179,8 +47656,14 @@
       <c r="D87" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>500</v>
       </c>
@@ -47193,8 +47676,14 @@
       <c r="D88" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>505</v>
       </c>
@@ -47207,8 +47696,14 @@
       <c r="D89" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>1868</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>509</v>
       </c>
@@ -47221,8 +47716,14 @@
       <c r="D90" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>513</v>
       </c>
@@ -47235,8 +47736,14 @@
       <c r="D91" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>515</v>
       </c>
@@ -47249,8 +47756,14 @@
       <c r="D92" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>519</v>
       </c>
@@ -47263,8 +47776,14 @@
       <c r="D93" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>523</v>
       </c>
@@ -47277,8 +47796,14 @@
       <c r="D94" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>527</v>
       </c>
@@ -47291,8 +47816,14 @@
       <c r="D95" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>532</v>
       </c>
@@ -47305,8 +47836,14 @@
       <c r="D96" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>533</v>
       </c>
@@ -47319,8 +47856,14 @@
       <c r="D97" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>537</v>
       </c>
@@ -47333,8 +47876,14 @@
       <c r="D98" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>542</v>
       </c>
@@ -47347,8 +47896,14 @@
       <c r="D99" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1419</v>
       </c>
@@ -47361,8 +47916,14 @@
       <c r="D100" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>550</v>
       </c>
@@ -47375,8 +47936,14 @@
       <c r="D101" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>554</v>
       </c>
@@ -47389,8 +47956,14 @@
       <c r="D102" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>558</v>
       </c>
@@ -47403,8 +47976,14 @@
       <c r="D103" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>565</v>
       </c>
@@ -47417,8 +47996,14 @@
       <c r="D104" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>569</v>
       </c>
@@ -47431,8 +48016,14 @@
       <c r="D105" t="s">
         <v>1422</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>578</v>
       </c>
@@ -47445,8 +48036,14 @@
       <c r="D106" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>582</v>
       </c>
@@ -47459,8 +48056,14 @@
       <c r="D107" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F107" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>588</v>
       </c>
@@ -47473,8 +48076,14 @@
       <c r="D108" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>592</v>
       </c>
@@ -47487,8 +48096,14 @@
       <c r="D109" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F109" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>599</v>
       </c>
@@ -47501,8 +48116,14 @@
       <c r="D110" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>604</v>
       </c>
@@ -47515,8 +48136,14 @@
       <c r="D111" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F111" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>614</v>
       </c>
@@ -47529,8 +48156,14 @@
       <c r="D112" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F112" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>619</v>
       </c>
@@ -47543,8 +48176,14 @@
       <c r="D113" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>623</v>
       </c>
@@ -47557,8 +48196,14 @@
       <c r="D114" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>630</v>
       </c>
@@ -47571,8 +48216,14 @@
       <c r="D115" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>634</v>
       </c>
@@ -47585,8 +48236,14 @@
       <c r="D116" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F116" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>640</v>
       </c>
@@ -47599,8 +48256,14 @@
       <c r="D117" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F117" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>649</v>
       </c>
@@ -47613,8 +48276,14 @@
       <c r="D118" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>653</v>
       </c>
@@ -47627,8 +48296,14 @@
       <c r="D119" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>657</v>
       </c>
@@ -47641,8 +48316,14 @@
       <c r="D120" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>663</v>
       </c>
@@ -47655,8 +48336,14 @@
       <c r="D121" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1430</v>
       </c>
@@ -47669,8 +48356,14 @@
       <c r="D122" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" t="s">
+        <v>1796</v>
+      </c>
+      <c r="F122" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>676</v>
       </c>
@@ -47683,8 +48376,14 @@
       <c r="D123" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>680</v>
       </c>
@@ -47697,8 +48396,14 @@
       <c r="D124" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>1798</v>
+      </c>
+      <c r="F124" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>689</v>
       </c>
@@ -47711,8 +48416,14 @@
       <c r="D125" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>1800</v>
+      </c>
+      <c r="F125" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>698</v>
       </c>
@@ -47725,8 +48436,14 @@
       <c r="D126" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>702</v>
       </c>
@@ -47739,8 +48456,14 @@
       <c r="D127" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>706</v>
       </c>
@@ -47753,8 +48476,14 @@
       <c r="D128" t="s">
         <v>1433</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>715</v>
       </c>
@@ -47767,8 +48496,14 @@
       <c r="D129" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>719</v>
       </c>
@@ -47781,8 +48516,14 @@
       <c r="D130" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>1804</v>
+      </c>
+      <c r="F130" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>728</v>
       </c>
@@ -47795,8 +48536,14 @@
       <c r="D131" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>1631</v>
+      </c>
+      <c r="F131" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>737</v>
       </c>
@@ -47809,8 +48556,14 @@
       <c r="D132" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F132" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>746</v>
       </c>
@@ -47823,8 +48576,14 @@
       <c r="D133" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>1808</v>
+      </c>
+      <c r="F133" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>755</v>
       </c>
@@ -47837,8 +48596,14 @@
       <c r="D134" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>759</v>
       </c>
@@ -47851,8 +48616,14 @@
       <c r="D135" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>1810</v>
+      </c>
+      <c r="F135" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>766</v>
       </c>
@@ -47865,8 +48636,14 @@
       <c r="D136" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>770</v>
       </c>
@@ -47879,8 +48656,14 @@
       <c r="D137" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>1812</v>
+      </c>
+      <c r="F137" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>779</v>
       </c>
@@ -47893,8 +48676,14 @@
       <c r="D138" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>1436</v>
       </c>
@@ -47907,8 +48696,14 @@
       <c r="D139" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>786</v>
       </c>
@@ -47921,8 +48716,14 @@
       <c r="D140" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" t="s">
+        <v>1814</v>
+      </c>
+      <c r="F140" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>795</v>
       </c>
@@ -47935,8 +48736,14 @@
       <c r="D141" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>799</v>
       </c>
@@ -47949,8 +48756,14 @@
       <c r="D142" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>803</v>
       </c>
@@ -47963,8 +48776,14 @@
       <c r="D143" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>807</v>
       </c>
@@ -47977,8 +48796,14 @@
       <c r="D144" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F144" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>814</v>
       </c>
@@ -47991,8 +48816,14 @@
       <c r="D145" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>818</v>
       </c>
@@ -48005,8 +48836,14 @@
       <c r="D146" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>823</v>
       </c>
@@ -48019,8 +48856,14 @@
       <c r="D147" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>1781</v>
+      </c>
+      <c r="F147" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>830</v>
       </c>
@@ -48033,8 +48876,14 @@
       <c r="D148" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>834</v>
       </c>
@@ -48047,8 +48896,14 @@
       <c r="D149" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>1818</v>
+      </c>
+      <c r="F149" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>841</v>
       </c>
@@ -48061,8 +48916,14 @@
       <c r="D150" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>845</v>
       </c>
@@ -48075,8 +48936,14 @@
       <c r="D151" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>1820</v>
+      </c>
+      <c r="F151" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>854</v>
       </c>
@@ -48089,8 +48956,14 @@
       <c r="D152" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>858</v>
       </c>
@@ -48103,8 +48976,14 @@
       <c r="D153" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>1442</v>
       </c>
@@ -48117,8 +48996,14 @@
       <c r="D154" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F154" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>867</v>
       </c>
@@ -48131,8 +49016,14 @@
       <c r="D155" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>871</v>
       </c>
@@ -48145,8 +49036,14 @@
       <c r="D156" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>875</v>
       </c>
@@ -48159,8 +49056,14 @@
       <c r="D157" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>879</v>
       </c>
@@ -48173,8 +49076,14 @@
       <c r="D158" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>883</v>
       </c>
@@ -48187,8 +49096,14 @@
       <c r="D159" t="s">
         <v>884</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F159" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>889</v>
       </c>
@@ -48201,8 +49116,14 @@
       <c r="D160" t="s">
         <v>1444</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" t="s">
+        <v>1768</v>
+      </c>
+      <c r="F160" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>897</v>
       </c>
@@ -48215,8 +49136,14 @@
       <c r="D161" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>902</v>
       </c>
@@ -48229,8 +49156,14 @@
       <c r="D162" t="s">
         <v>1446</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F162" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>909</v>
       </c>
@@ -48243,8 +49176,14 @@
       <c r="D163" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>913</v>
       </c>
@@ -48257,8 +49196,14 @@
       <c r="D164" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" t="s">
+        <v>1757</v>
+      </c>
+      <c r="F164" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>920</v>
       </c>
@@ -48271,8 +49216,14 @@
       <c r="D165" t="s">
         <v>924</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F165" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>928</v>
       </c>
@@ -48285,8 +49236,14 @@
       <c r="D166" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166">
+        <v>0</v>
+      </c>
+      <c r="F166" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>932</v>
       </c>
@@ -48299,8 +49256,14 @@
       <c r="D167" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="F167" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>936</v>
       </c>
@@ -48313,8 +49276,14 @@
       <c r="D168" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="F168" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>940</v>
       </c>
@@ -48327,8 +49296,14 @@
       <c r="D169" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="F169" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>945</v>
       </c>
@@ -48341,8 +49316,14 @@
       <c r="D170" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>950</v>
       </c>
@@ -48355,8 +49336,14 @@
       <c r="D171" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>954</v>
       </c>
@@ -48369,8 +49356,14 @@
       <c r="D172" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>958</v>
       </c>
@@ -48383,8 +49376,14 @@
       <c r="D173" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F173" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>964</v>
       </c>
@@ -48397,8 +49396,14 @@
       <c r="D174" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>968</v>
       </c>
@@ -48411,8 +49416,14 @@
       <c r="D175" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>972</v>
       </c>
@@ -48425,8 +49436,14 @@
       <c r="D176" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F176" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>978</v>
       </c>
@@ -48439,8 +49456,14 @@
       <c r="D177" t="s">
         <v>982</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F177" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>987</v>
       </c>
@@ -48453,8 +49476,14 @@
       <c r="D178" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>992</v>
       </c>
@@ -48467,8 +49496,14 @@
       <c r="D179" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>996</v>
       </c>
@@ -48481,8 +49516,14 @@
       <c r="D180" t="s">
         <v>1000</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F180" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>1004</v>
       </c>
@@ -48495,8 +49536,14 @@
       <c r="D181" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>1008</v>
       </c>
@@ -48509,8 +49556,14 @@
       <c r="D182" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>1012</v>
       </c>
@@ -48523,8 +49576,14 @@
       <c r="D183" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>1016</v>
       </c>
@@ -48537,8 +49596,14 @@
       <c r="D184" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>1020</v>
       </c>
@@ -48551,22 +49616,34 @@
       <c r="D185" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>1024</v>
       </c>
       <c r="B186" t="s">
-        <v>1882</v>
+        <v>1454</v>
       </c>
       <c r="C186" t="s">
         <v>1666</v>
       </c>
       <c r="D186" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1455</v>
+      </c>
+      <c r="E186" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F186" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>1031</v>
       </c>
@@ -48579,8 +49656,14 @@
       <c r="D187" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F187" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>1456</v>
       </c>
@@ -48593,8 +49676,14 @@
       <c r="D188" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F188" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>1044</v>
       </c>
@@ -48607,8 +49696,14 @@
       <c r="D189" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>1048</v>
       </c>
@@ -48621,8 +49716,14 @@
       <c r="D190" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>1052</v>
       </c>
@@ -48635,8 +49736,14 @@
       <c r="D191" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>1056</v>
       </c>
@@ -48649,8 +49756,14 @@
       <c r="D192" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>1058</v>
       </c>
@@ -48663,8 +49776,14 @@
       <c r="D193" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193">
+        <v>0</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>1062</v>
       </c>
@@ -48677,8 +49796,14 @@
       <c r="D194" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194">
+        <v>0</v>
+      </c>
+      <c r="F194" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>1066</v>
       </c>
@@ -48691,8 +49816,14 @@
       <c r="D195" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>1070</v>
       </c>
@@ -48705,8 +49836,14 @@
       <c r="D196" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>1074</v>
       </c>
@@ -48719,8 +49856,14 @@
       <c r="D197" t="s">
         <v>1078</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F197" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>1083</v>
       </c>
@@ -48733,8 +49876,14 @@
       <c r="D198" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198">
+        <v>0</v>
+      </c>
+      <c r="F198" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>1087</v>
       </c>
@@ -48747,8 +49896,14 @@
       <c r="D199" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199">
+        <v>0</v>
+      </c>
+      <c r="F199" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>1092</v>
       </c>
@@ -48761,8 +49916,14 @@
       <c r="D200" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200">
+        <v>0</v>
+      </c>
+      <c r="F200" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>1096</v>
       </c>
@@ -48775,8 +49936,14 @@
       <c r="D201" t="s">
         <v>1099</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F201" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>1104</v>
       </c>
@@ -48789,8 +49956,14 @@
       <c r="D202" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202">
+        <v>0</v>
+      </c>
+      <c r="F202" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>1108</v>
       </c>
@@ -48803,8 +49976,14 @@
       <c r="D203" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203">
+        <v>0</v>
+      </c>
+      <c r="F203" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>1112</v>
       </c>
@@ -48817,8 +49996,14 @@
       <c r="D204" t="s">
         <v>1116</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>1117</v>
       </c>
@@ -48831,8 +50016,14 @@
       <c r="D205" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205">
+        <v>0</v>
+      </c>
+      <c r="F205" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>1122</v>
       </c>
@@ -48845,8 +50036,14 @@
       <c r="D206" t="s">
         <v>1126</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F206" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>1131</v>
       </c>
@@ -48859,8 +50056,14 @@
       <c r="D207" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207">
+        <v>0</v>
+      </c>
+      <c r="F207" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>1135</v>
       </c>
@@ -48873,8 +50076,14 @@
       <c r="D208" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208">
+        <v>0</v>
+      </c>
+      <c r="F208" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>1139</v>
       </c>
@@ -48887,8 +50096,14 @@
       <c r="D209" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209">
+        <v>0</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>1143</v>
       </c>
@@ -48901,13 +50116,19 @@
       <c r="D210" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210">
+        <v>0</v>
+      </c>
+      <c r="F210" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>1147</v>
       </c>
       <c r="B211" t="s">
-        <v>1881</v>
+        <v>1466</v>
       </c>
       <c r="C211" t="s">
         <v>1691</v>
@@ -48915,8 +50136,14 @@
       <c r="D211" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211">
+        <v>0</v>
+      </c>
+      <c r="F211" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>1151</v>
       </c>
@@ -48929,13 +50156,19 @@
       <c r="D212" t="s">
         <v>1155</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" t="s">
+        <v>1842</v>
+      </c>
+      <c r="F212" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>1160</v>
       </c>
       <c r="B213" t="s">
-        <v>1880</v>
+        <v>1467</v>
       </c>
       <c r="C213" t="s">
         <v>1693</v>
@@ -48943,8 +50176,14 @@
       <c r="D213" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213">
+        <v>0</v>
+      </c>
+      <c r="F213" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>1468</v>
       </c>
@@ -48957,8 +50196,14 @@
       <c r="D214" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214">
+        <v>0</v>
+      </c>
+      <c r="F214" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>1168</v>
       </c>
@@ -48971,8 +50216,14 @@
       <c r="D215" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215">
+        <v>0</v>
+      </c>
+      <c r="F215" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>1172</v>
       </c>
@@ -48985,8 +50236,14 @@
       <c r="D216" t="s">
         <v>1091</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216">
+        <v>0</v>
+      </c>
+      <c r="F216" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>1176</v>
       </c>
@@ -48999,8 +50256,14 @@
       <c r="D217" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217">
+        <v>0</v>
+      </c>
+      <c r="F217" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>1180</v>
       </c>
@@ -49013,8 +50276,14 @@
       <c r="D218" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218">
+        <v>0</v>
+      </c>
+      <c r="F218" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>1184</v>
       </c>
@@ -49027,8 +50296,14 @@
       <c r="D219" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" t="s">
+        <v>1785</v>
+      </c>
+      <c r="F219" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>1192</v>
       </c>
@@ -49041,8 +50316,14 @@
       <c r="D220" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" t="s">
+        <v>1845</v>
+      </c>
+      <c r="F220" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>1202</v>
       </c>
@@ -49055,8 +50336,14 @@
       <c r="D221" t="s">
         <v>1470</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F221" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>1471</v>
       </c>
@@ -49069,8 +50356,14 @@
       <c r="D222" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222">
+        <v>0</v>
+      </c>
+      <c r="F222" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>1213</v>
       </c>
@@ -49083,8 +50376,14 @@
       <c r="D223" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" t="s">
+        <v>1582</v>
+      </c>
+      <c r="F223" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>1220</v>
       </c>
@@ -49097,8 +50396,14 @@
       <c r="D224" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224">
+        <v>0</v>
+      </c>
+      <c r="F224" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>1224</v>
       </c>
@@ -49111,8 +50416,14 @@
       <c r="D225" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225">
+        <v>0</v>
+      </c>
+      <c r="F225" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>1229</v>
       </c>
@@ -49125,8 +50436,14 @@
       <c r="D226" t="s">
         <v>1233</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226">
+        <v>0</v>
+      </c>
+      <c r="F226" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>1234</v>
       </c>
@@ -49139,8 +50456,14 @@
       <c r="D227" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227">
+        <v>0</v>
+      </c>
+      <c r="F227" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>1238</v>
       </c>
@@ -49153,8 +50476,14 @@
       <c r="D228" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228">
+        <v>0</v>
+      </c>
+      <c r="F228" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>1239</v>
       </c>
@@ -49167,8 +50496,14 @@
       <c r="D229" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229">
+        <v>0</v>
+      </c>
+      <c r="F229" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>1243</v>
       </c>
@@ -49181,8 +50516,14 @@
       <c r="D230" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230">
+        <v>0</v>
+      </c>
+      <c r="F230" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>1247</v>
       </c>
@@ -49195,8 +50536,14 @@
       <c r="D231" t="s">
         <v>1251</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F231" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>1256</v>
       </c>
@@ -49209,8 +50556,14 @@
       <c r="D232" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232">
+        <v>0</v>
+      </c>
+      <c r="F232" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>1260</v>
       </c>
@@ -49221,10 +50574,16 @@
         <v>1712</v>
       </c>
       <c r="D233" t="s">
-        <v>1879</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1475</v>
+      </c>
+      <c r="E233" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F233" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>1269</v>
       </c>
@@ -49237,8 +50596,14 @@
       <c r="D234" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="F234" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>1273</v>
       </c>
@@ -49251,8 +50616,14 @@
       <c r="D235" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235">
+        <v>0</v>
+      </c>
+      <c r="F235" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>1276</v>
       </c>
@@ -49265,8 +50636,14 @@
       <c r="D236" t="s">
         <v>1277</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" t="s">
+        <v>1595</v>
+      </c>
+      <c r="F236" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>1280</v>
       </c>
@@ -49279,8 +50656,14 @@
       <c r="D237" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E237" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F237" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>1287</v>
       </c>
@@ -49293,8 +50676,14 @@
       <c r="D238" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E238">
+        <v>0</v>
+      </c>
+      <c r="F238" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>1292</v>
       </c>
@@ -49307,22 +50696,34 @@
       <c r="D239" t="s">
         <v>1296</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E239" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F239" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>1299</v>
       </c>
       <c r="B240" t="s">
-        <v>1876</v>
+        <v>1477</v>
       </c>
       <c r="C240" t="s">
         <v>1717</v>
       </c>
       <c r="D240" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1478</v>
+      </c>
+      <c r="E240" t="s">
+        <v>1856</v>
+      </c>
+      <c r="F240" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>1308</v>
       </c>
@@ -49335,8 +50736,14 @@
       <c r="D241" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E241">
+        <v>0</v>
+      </c>
+      <c r="F241" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>1312</v>
       </c>
@@ -49349,8 +50756,14 @@
       <c r="D242" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E242">
+        <v>0</v>
+      </c>
+      <c r="F242" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>1316</v>
       </c>
@@ -49361,10 +50774,16 @@
         <v>1720</v>
       </c>
       <c r="D243" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1479</v>
+      </c>
+      <c r="E243" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F243" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>1325</v>
       </c>
@@ -49377,8 +50796,14 @@
       <c r="D244" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E244">
+        <v>0</v>
+      </c>
+      <c r="F244" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>1329</v>
       </c>
@@ -49391,8 +50816,14 @@
       <c r="D245" t="s">
         <v>1333</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E245" t="s">
+        <v>1860</v>
+      </c>
+      <c r="F245" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>1338</v>
       </c>
@@ -49405,8 +50836,14 @@
       <c r="D246" t="s">
         <v>1342</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F246" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>1345</v>
       </c>
@@ -49419,8 +50856,14 @@
       <c r="D247" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247">
+        <v>0</v>
+      </c>
+      <c r="F247" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>1347</v>
       </c>
@@ -49433,8 +50876,14 @@
       <c r="D248" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248">
+        <v>0</v>
+      </c>
+      <c r="F248" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>1351</v>
       </c>
@@ -49447,8 +50896,14 @@
       <c r="D249" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E249">
+        <v>0</v>
+      </c>
+      <c r="F249" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>1355</v>
       </c>
@@ -49461,8 +50916,14 @@
       <c r="D250" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250">
+        <v>0</v>
+      </c>
+      <c r="F250" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>1359</v>
       </c>
@@ -49475,8 +50936,14 @@
       <c r="D251" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251">
+        <v>0</v>
+      </c>
+      <c r="F251" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>1363</v>
       </c>
@@ -49489,8 +50956,14 @@
       <c r="D252" t="s">
         <v>1367</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E252" t="s">
+        <v>1863</v>
+      </c>
+      <c r="F252" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>1372</v>
       </c>
@@ -49503,22 +50976,35 @@
       <c r="D253" t="s">
         <v>1484</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253" t="s">
+        <v>1865</v>
+      </c>
+      <c r="F253" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>1381</v>
       </c>
       <c r="B254" t="s">
-        <v>1874</v>
+        <v>1397</v>
       </c>
       <c r="C254" t="s">
         <v>1536</v>
       </c>
       <c r="D254" t="s">
-        <v>1875</v>
+        <v>1425</v>
+      </c>
+      <c r="E254" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F254" t="s">
+        <v>1867</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>